<commit_message>
Se corrige el resultado anterior.
El informe no incluía los datos de pactos del día de hoy.
</commit_message>
<xml_diff>
--- a/Nevasa/InformeCompleto/20240904/20240904_informe_completo_results.xlsx
+++ b/Nevasa/InformeCompleto/20240904/20240904_informe_completo_results.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -816,36 +816,36 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>45539</v>
+        <v>45540</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>45539</v>
       </c>
       <c r="D10" t="n">
-        <v>5.4</v>
+        <v>0.48</v>
       </c>
       <c r="E10" t="n">
-        <v>500000000</v>
+        <v>22003520</v>
       </c>
       <c r="F10" t="n">
-        <v>522623709</v>
+        <v>22000000</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>BTP0581029</t>
+          <t>PACTO</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>VENTA</t>
+          <t>COMPRA</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>RENTA FIJA</t>
+          <t>PACTO</t>
         </is>
       </c>
     </row>
@@ -862,20 +862,20 @@
         <v>45539</v>
       </c>
       <c r="D11" t="n">
-        <v>5.87</v>
+        <v>5.4</v>
       </c>
       <c r="E11" t="n">
-        <v>2000000000</v>
+        <v>500000000</v>
       </c>
       <c r="F11" t="n">
-        <v>1900159321</v>
+        <v>522623709</v>
       </c>
       <c r="G11" t="n">
         <v>0</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>BBCIO21220</t>
+          <t>BTP0581029</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -902,20 +902,20 @@
         <v>45539</v>
       </c>
       <c r="D12" t="n">
-        <v>3.6</v>
+        <v>5.87</v>
       </c>
       <c r="E12" t="n">
-        <v>5000</v>
+        <v>2000000000</v>
       </c>
       <c r="F12" t="n">
-        <v>192289952</v>
+        <v>1900159321</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>BCAJBF0322</t>
+          <t>BBCIO21220</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -942,20 +942,20 @@
         <v>45539</v>
       </c>
       <c r="D13" t="n">
-        <v>5.85</v>
+        <v>3.6</v>
       </c>
       <c r="E13" t="n">
-        <v>500000000</v>
+        <v>5000</v>
       </c>
       <c r="F13" t="n">
-        <v>488642906</v>
+        <v>192289952</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>BCHIDU0716</t>
+          <t>BCAJBF0322</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -982,25 +982,25 @@
         <v>45539</v>
       </c>
       <c r="D14" t="n">
-        <v>2.36</v>
+        <v>5.85</v>
       </c>
       <c r="E14" t="n">
-        <v>23000</v>
+        <v>500000000</v>
       </c>
       <c r="F14" t="n">
-        <v>900457256</v>
+        <v>488642906</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>BCHIAZ0613</t>
+          <t>BCHIDU0716</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>COMPRA</t>
+          <t>VENTA</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1022,20 +1022,20 @@
         <v>45539</v>
       </c>
       <c r="D15" t="n">
-        <v>2.06</v>
+        <v>2.36</v>
       </c>
       <c r="E15" t="n">
-        <v>1000</v>
+        <v>23000</v>
       </c>
       <c r="F15" t="n">
-        <v>38066280</v>
+        <v>900457256</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>BSECK70915</t>
+          <t>BCHIAZ0613</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1062,13 +1062,13 @@
         <v>45539</v>
       </c>
       <c r="D16" t="n">
-        <v>2.05</v>
+        <v>2.06</v>
       </c>
       <c r="E16" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="F16" t="n">
-        <v>76139894</v>
+        <v>38066280</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -1102,30 +1102,350 @@
         <v>45539</v>
       </c>
       <c r="D17" t="n">
-        <v>0</v>
+        <v>2.05</v>
       </c>
       <c r="E17" t="n">
+        <v>2000</v>
+      </c>
+      <c r="F17" t="n">
+        <v>76139894</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>BSECK70915</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>COMPRA</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>RENTA FIJA</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>45539</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>45539</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F18" t="n">
+        <v>38059258</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>BSECK70915</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>COMPRA</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>RENTA FIJA</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>45539</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>45539</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="E19" t="n">
+        <v>30000</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1132814474</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>BBNSAN0918</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>COMPRA</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>RENTA FIJA</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>45539</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>45539</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="E20" t="n">
+        <v>30000</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1169147129</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>BCODE-B</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>COMPRA</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>RENTA FIJA</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>45539</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>45539</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
         <v>18044822.5</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F21" t="n">
         <v>18037764</v>
       </c>
-      <c r="G17" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" t="inlineStr">
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" t="inlineStr">
         <is>
           <t>SQM-B</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>VENTA</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>SIMULTANEA</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>45539</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>45539</v>
+      </c>
+      <c r="D22" t="n">
+        <v>16425</v>
+      </c>
+      <c r="E22" t="n">
+        <v>919</v>
+      </c>
+      <c r="F22" t="n">
+        <v>15094575</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>CFINHRFLA</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>COMPRA</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>RENTA VARIABLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>45539</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>45539</v>
+      </c>
+      <c r="D23" t="n">
+        <v>16425.05</v>
+      </c>
+      <c r="E23" t="n">
+        <v>147</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2414483</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>CFINHRFLA</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>COMPRA</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>RENTA VARIABLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>45539</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>45539</v>
+      </c>
+      <c r="D24" t="n">
+        <v>16425.05</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1091</v>
+      </c>
+      <c r="F24" t="n">
+        <v>17919730</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>CFINHRFLA</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>VENTA</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>RENTA VARIABLE</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>FONDO DE INVERSION NEVASA AHORRO</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>45539</v>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>45539</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1183.88</v>
+      </c>
+      <c r="E25" t="n">
+        <v>2535</v>
+      </c>
+      <c r="F25" t="n">
+        <v>3001136</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>CFINVRFLI</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>COMPRA</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>RENTA VARIABLE</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrección en la lógica de compra de simultaneas
</commit_message>
<xml_diff>
--- a/Nevasa/InformeCompleto/20240904/20240904_informe_completo_results.xlsx
+++ b/Nevasa/InformeCompleto/20240904/20240904_informe_completo_results.xlsx
@@ -505,10 +505,10 @@
         <v>0.61</v>
       </c>
       <c r="E2" t="n">
+        <v>38290936</v>
+      </c>
+      <c r="F2" t="n">
         <v>38074100</v>
-      </c>
-      <c r="F2" t="n">
-        <v>38290936</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -545,10 +545,10 @@
         <v>0.53</v>
       </c>
       <c r="E3" t="n">
+        <v>75823500</v>
+      </c>
+      <c r="F3" t="n">
         <v>74250000</v>
-      </c>
-      <c r="F3" t="n">
-        <v>75823500</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
@@ -585,10 +585,10 @@
         <v>0.54</v>
       </c>
       <c r="E4" t="n">
+        <v>75853500</v>
+      </c>
+      <c r="F4" t="n">
         <v>74250000</v>
-      </c>
-      <c r="F4" t="n">
-        <v>75853500</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -625,10 +625,10 @@
         <v>0.53</v>
       </c>
       <c r="E5" t="n">
+        <v>76590000</v>
+      </c>
+      <c r="F5" t="n">
         <v>75000000</v>
-      </c>
-      <c r="F5" t="n">
-        <v>76590000</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -665,10 +665,10 @@
         <v>0.53</v>
       </c>
       <c r="E6" t="n">
+        <v>36762000</v>
+      </c>
+      <c r="F6" t="n">
         <v>36000000</v>
-      </c>
-      <c r="F6" t="n">
-        <v>36762000</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -705,10 +705,10 @@
         <v>0.55</v>
       </c>
       <c r="E7" t="n">
+        <v>76036800</v>
+      </c>
+      <c r="F7" t="n">
         <v>74400000</v>
-      </c>
-      <c r="F7" t="n">
-        <v>76036800</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -745,10 +745,10 @@
         <v>0.58</v>
       </c>
       <c r="E8" t="n">
+        <v>12123481</v>
+      </c>
+      <c r="F8" t="n">
         <v>12021300</v>
-      </c>
-      <c r="F8" t="n">
-        <v>12123481</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -785,10 +785,10 @@
         <v>0.55</v>
       </c>
       <c r="E9" t="n">
+        <v>109170040</v>
+      </c>
+      <c r="F9" t="n">
         <v>106820000</v>
-      </c>
-      <c r="F9" t="n">
-        <v>109170040</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>

</xml_diff>